<commit_message>
added Alexandre inside Git
</commit_message>
<xml_diff>
--- a/doc/gant.xlsx
+++ b/doc/gant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="380" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>RO</t>
   </si>
   <si>
-    <t>IHM</t>
-  </si>
-  <si>
     <t>LW</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Intégration</t>
+  </si>
+  <si>
+    <t>IHM / Alexandre</t>
   </si>
 </sst>
 </file>
@@ -179,13 +179,13 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -522,7 +522,7 @@
   <dimension ref="A3:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -538,10 +538,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>5</v>
@@ -563,7 +563,7 @@
       <c r="D4" s="1">
         <v>42253</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:10">
       <c r="B5">
@@ -575,9 +575,9 @@
       <c r="D5" s="1">
         <v>42260</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:10">
@@ -590,11 +590,11 @@
       <c r="D6" s="1">
         <v>42267</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="11"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:10">
@@ -607,11 +607,11 @@
       <c r="D7" s="1">
         <v>42274</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>8</v>
+      <c r="E7" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:10">
@@ -624,11 +624,11 @@
       <c r="D8" s="1">
         <v>42281</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>9</v>
+      <c r="E8" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:10">
@@ -641,12 +641,12 @@
       <c r="D9" s="1">
         <v>42288</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>10</v>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="12" t="s">
-        <v>12</v>
+      <c r="G9" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -661,7 +661,7 @@
         <v>42295</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
@@ -676,11 +676,11 @@
         <v>42302</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="11"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="4">
@@ -694,7 +694,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="10"/>
+      <c r="A13" s="14"/>
       <c r="B13">
         <v>45</v>
       </c>
@@ -705,29 +705,29 @@
         <v>42316</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12">
+        <v>46</v>
+      </c>
+      <c r="C14" s="13">
+        <v>42317</v>
+      </c>
+      <c r="D14" s="13">
+        <v>42323</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" t="s">
         <v>13</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13">
-        <v>46</v>
-      </c>
-      <c r="C14" s="14">
-        <v>42317</v>
-      </c>
-      <c r="D14" s="14">
-        <v>42323</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -741,7 +741,7 @@
         <v>42330</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="11"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:10">
@@ -755,7 +755,7 @@
         <v>42337</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="11"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:7">
@@ -769,11 +769,11 @@
         <v>42344</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1">
       <c r="A18" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="8">
         <v>50</v>
@@ -800,7 +800,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="4" customFormat="1">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="4">
@@ -814,7 +814,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1">
-      <c r="A21" s="10"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4">
         <v>1</v>
       </c>
@@ -879,7 +879,6 @@
     <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>